<commit_message>
replaced ContributionSpreadsheet.xlsx template with filled out version for code review 1
</commit_message>
<xml_diff>
--- a/Documentation/ContributionSpreadsheet.xlsx
+++ b/Documentation/ContributionSpreadsheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livenapierac-my.sharepoint.com/personal/40646660_live_napier_ac_uk/Documents/Software Engineering Methods/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebek\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC68904C-50CB-4CC9-982B-376CA71E598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347B3FFB-D49C-4F89-B1C8-808F6F414B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{CC6A97E2-76B9-4223-B2A9-CBFF6BB7AA4C}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="13152" windowHeight="8880" xr2:uid="{CC6A97E2-76B9-4223-B2A9-CBFF6BB7AA4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -298,7 +299,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -311,6 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -329,9 +330,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -369,7 +370,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -475,7 +476,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,7 +629,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,12 +641,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
@@ -682,115 +683,123 @@
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>40646650</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11">
+      <c r="C8" s="5">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="10">
         <f>SUM(C8:F8)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>40716597</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11">
+      <c r="C9" s="5">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10">
         <f t="shared" ref="G9:G11" si="0">SUM(C9:F9)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>40646660</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11">
+      <c r="C10" s="5">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>40646671</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="11">
+      <c r="C11" s="9">
+        <v>25</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <f>SUM(C8:C11)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="11">
+        <v>100</v>
+      </c>
+      <c r="D12" s="10">
         <f t="shared" ref="D12:F12" si="1">SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -809,6 +818,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002B186A1A0ED80C43A714C20B4190D02C" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41e08d578e13f4c671c6c9ebf4131a2b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="99914f43-2249-453f-9e90-9cf89711f5cd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d73df9724357b65cc5edaf353590e019" ns3:_="">
     <xsd:import namespace="99914f43-2249-453f-9e90-9cf89711f5cd"/>
@@ -958,15 +976,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -974,6 +983,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6FCECC7-06AC-4706-8D9A-7678216FB06A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE0EED37-36B2-459E-B427-6966AB68DA37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -987,14 +1004,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6FCECC7-06AC-4706-8D9A-7678216FB06A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>